<commit_message>
log log model structure
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\166.2.126.25\rseat\Programs\Reimbursibles\fy2016\R3_lidar_equation_transferability\Analysis\VersionControl\lidarNew\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krtenneson\Desktop\lidarPaper\lidarNew\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
   <si>
     <t>Model no weights</t>
   </si>
@@ -65,9 +65,6 @@
     <t>no 0</t>
   </si>
   <si>
-    <t>fit with zeroes</t>
-  </si>
-  <si>
     <t>38.8+25</t>
   </si>
   <si>
@@ -126,6 +123,18 @@
   </si>
   <si>
     <t>43.4+20.3</t>
+  </si>
+  <si>
+    <t>log, log fit with zeroes</t>
+  </si>
+  <si>
+    <t>log, fit with zeroes</t>
+  </si>
+  <si>
+    <t>39.5 + 21.3</t>
+  </si>
+  <si>
+    <t>40.145+19.6</t>
   </si>
 </sst>
 </file>
@@ -134,7 +143,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -316,11 +325,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -329,7 +338,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -345,20 +354,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -366,21 +366,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -662,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,48 +684,59 @@
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11"/>
-      <c r="C1" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20" t="s">
+      <c r="C1" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="38"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="21"/>
-    </row>
-    <row r="2" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="39"/>
+    </row>
+    <row r="2" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31" t="s">
+      <c r="H2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="32"/>
-    </row>
-    <row r="3" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="41"/>
+    </row>
+    <row r="3" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="C3" s="13" t="s">
         <v>9</v>
@@ -723,26 +744,32 @@
       <c r="D3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="H3" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="I3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="33" t="s">
+      <c r="J3" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="33" t="s">
+      <c r="K3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="34" t="s">
+      <c r="L3" s="29" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
@@ -751,14 +778,16 @@
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="36"/>
-    </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="15"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="31"/>
+    </row>
+    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
         <v>6</v>
@@ -769,60 +798,66 @@
       <c r="D5" s="3">
         <v>29047</v>
       </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="37">
+      <c r="E5" s="16"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="32">
         <v>28881.56</v>
       </c>
-      <c r="H5" s="37">
+      <c r="J5" s="32">
         <v>28881.56</v>
       </c>
-      <c r="I5" s="37"/>
-      <c r="J5" s="38">
+      <c r="K5" s="32"/>
+      <c r="L5" s="33">
         <v>28882</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="39">
+      <c r="C6" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="21"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="34">
         <v>37.700000000000003</v>
       </c>
-      <c r="G6" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="26"/>
-      <c r="J6" s="39" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I6" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="23"/>
+      <c r="L6" s="34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="5"/>
       <c r="C7" s="18"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="41"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E7" s="18"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="36"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -831,14 +866,16 @@
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="36"/>
-    </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="15"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="31"/>
+    </row>
+    <row r="9" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="3" t="s">
         <v>6</v>
@@ -849,56 +886,62 @@
       <c r="D9" s="3">
         <v>29732</v>
       </c>
-      <c r="E9" s="37"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37">
+      <c r="E9" s="16"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32">
         <v>29611</v>
       </c>
-      <c r="I9" s="37"/>
-      <c r="J9" s="38">
+      <c r="K9" s="32"/>
+      <c r="L9" s="33">
         <v>29593</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="39">
+        <v>18</v>
+      </c>
+      <c r="E10" s="17"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="34">
         <v>39.5</v>
       </c>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="I10" s="26"/>
-      <c r="J10" s="39" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I10" s="23"/>
+      <c r="J10" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" s="23"/>
+      <c r="L10" s="34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="5"/>
       <c r="C11" s="18"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="41"/>
-    </row>
-    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E11" s="18"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="36"/>
+    </row>
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>2</v>
       </c>
@@ -907,74 +950,90 @@
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="36"/>
-    </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="15"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="31"/>
+    </row>
+    <row r="13" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="20">
         <v>9505</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="19">
         <v>9505</v>
       </c>
-      <c r="E13" s="37"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37">
+      <c r="E13" s="20">
+        <v>8889.5</v>
+      </c>
+      <c r="F13" s="19">
+        <v>8862.9549999999999</v>
+      </c>
+      <c r="G13" s="32"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32">
         <v>7939</v>
       </c>
-      <c r="I13" s="37"/>
-      <c r="J13" s="38">
+      <c r="K13" s="32"/>
+      <c r="L13" s="33">
         <v>7936</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="39">
+      <c r="C14" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="34">
         <v>36.799999999999997</v>
       </c>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="I14" s="26"/>
-      <c r="J14" s="39" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I14" s="23"/>
+      <c r="J14" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="K14" s="23"/>
+      <c r="L14" s="34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="5"/>
       <c r="C15" s="18"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="41"/>
-    </row>
-    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E15" s="18"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="36"/>
+    </row>
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>3</v>
       </c>
@@ -983,14 +1042,16 @@
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="36"/>
-    </row>
-    <row r="17" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="15"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="31"/>
+    </row>
+    <row r="17" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="3" t="s">
         <v>6</v>
@@ -1001,56 +1062,62 @@
       <c r="D17" s="3">
         <v>10126</v>
       </c>
-      <c r="E17" s="37"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37">
+      <c r="E17" s="16"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32">
         <v>8925.2000000000007</v>
       </c>
-      <c r="I17" s="37"/>
-      <c r="J17" s="38">
+      <c r="K17" s="32"/>
+      <c r="L17" s="33">
         <v>8866</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="39">
+        <v>19</v>
+      </c>
+      <c r="E18" s="17"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="34">
         <v>47.2</v>
       </c>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="I18" s="26"/>
-      <c r="J18" s="39" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I18" s="23"/>
+      <c r="J18" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K18" s="23"/>
+      <c r="L18" s="34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="5"/>
       <c r="C19" s="18"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="41"/>
-    </row>
-    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E19" s="18"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="36"/>
+    </row>
+    <row r="20" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>4</v>
       </c>
@@ -1059,14 +1126,16 @@
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="36"/>
-    </row>
-    <row r="21" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="15"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="31"/>
+    </row>
+    <row r="21" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="3" t="s">
         <v>6</v>
@@ -1077,49 +1146,54 @@
       <c r="D21" s="3">
         <v>10470</v>
       </c>
-      <c r="E21" s="37"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37">
+      <c r="E21" s="16"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32">
         <v>8974</v>
       </c>
-      <c r="I21" s="37"/>
-      <c r="J21" s="38">
+      <c r="K21" s="32"/>
+      <c r="L21" s="33">
         <v>8957</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" s="41">
+        <v>17</v>
+      </c>
+      <c r="E22" s="18"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" s="36">
         <v>43.4</v>
       </c>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="I22" s="40"/>
-      <c r="J22" s="41" t="s">
-        <v>25</v>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="K22" s="35"/>
+      <c r="L22" s="36" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="G2:H2"/>
+  <mergeCells count="5">
+    <mergeCell ref="I1:L1"/>
     <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>